<commit_message>
Envio dos email repetidos
</commit_message>
<xml_diff>
--- a/excel/teste_faturamento-teste-email-duplicado 1.xlsx
+++ b/excel/teste_faturamento-teste-email-duplicado 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27021"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mescobar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0CC8F95-29AF-4143-A4BD-13EC80415AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F7EA868-3C06-4DF3-A47C-2AB4F999A664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C7440688-394F-4B73-A8BB-FC087BB8E5CF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="343">
   <si>
     <t>ID interno</t>
   </si>
@@ -116,9 +116,6 @@
     <t>LOJA BK PARNAÍBA, BKN 26203  -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS  REF SETEMBRO</t>
   </si>
   <si>
-    <t>phnovaisnew@outlook.com</t>
-  </si>
-  <si>
     <t>1172 MICHEF COMERCIO DE ALIMENTOS LTDA - EPP</t>
   </si>
   <si>
@@ -170,7 +167,7 @@
     <t>MATOS E KRETLI- BKN 27721 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
   </si>
   <si>
-    <t>bkto27721@gmail.com</t>
+    <t>teste@gmail.com</t>
   </si>
   <si>
     <t>012456</t>
@@ -185,9 +182,6 @@
     <t>LOJA RONDONÓLIS BKN 27968, MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
   </si>
   <si>
-    <t>contab.karla@estreladistribuidora.com.br</t>
-  </si>
-  <si>
     <t>012457</t>
   </si>
   <si>
@@ -212,766 +206,766 @@
     <t>LOJA ITABUNA BKN 27985  - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
   </si>
   <si>
+    <t>012459</t>
+  </si>
+  <si>
+    <t>1673 CAMPOS CHAVES PRODUTOS ALIMENTICIOS LTDA</t>
+  </si>
+  <si>
+    <t>34.798.861/0001-89</t>
+  </si>
+  <si>
+    <t>LOJA GOVERNADOR VALADARES, BKN 27996 -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>setorfinanceiro.uniao@gmail.com</t>
+  </si>
+  <si>
+    <t>012460</t>
+  </si>
+  <si>
+    <t>1659 CONFORTI COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>26.390.660/0006-24</t>
+  </si>
+  <si>
+    <t>LOJA CAMPO GRANDE - MT  BKN 27986 -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>financeiro@bkconforti.com</t>
+  </si>
+  <si>
+    <t>012461</t>
+  </si>
+  <si>
+    <t>1665 RCPM ALIMENTACAO LTDA</t>
+  </si>
+  <si>
+    <t>34.854.503/0001-46</t>
+  </si>
+  <si>
+    <t>LOJA OIAPOQUE BKN 25048 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>ricardo.de.campos@hotmail.com</t>
+  </si>
+  <si>
+    <t>012462</t>
+  </si>
+  <si>
+    <t>1597 BK BLESS COMERCIO DE ALIMENTOS EIRELI</t>
+  </si>
+  <si>
+    <t>34.911.443/0003-18</t>
+  </si>
+  <si>
+    <t>LOJA ZAFFARI HÍPICA BKN 27993- MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>financeiro.bk@empresasbless.com.br</t>
+  </si>
+  <si>
+    <t>012463</t>
+  </si>
+  <si>
+    <t>1667 BK BLESS COMERCIO DE ALIMENTOS EIRELI</t>
+  </si>
+  <si>
+    <t>34.911.443/0002-37</t>
+  </si>
+  <si>
+    <t>LOJA JOÃO PESSOA SHOPPING BKN 27992 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012464</t>
+  </si>
+  <si>
+    <t>1686 3A LANCHONETE LTDA</t>
+  </si>
+  <si>
+    <t>34.953.955/0001-85</t>
+  </si>
+  <si>
+    <t>ALPHA SHOPPING BKN 27592 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>alphashopping.bk@gmail.com</t>
+  </si>
+  <si>
+    <t>012465</t>
+  </si>
+  <si>
+    <t>1676 ELM COMÉRCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>35.561.003/0001-89</t>
+  </si>
+  <si>
+    <t>LOJA GREEN PLAZA - MG  BKN 28227 MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>bkgreenplaza@gmail.com</t>
+  </si>
+  <si>
+    <t>012466</t>
+  </si>
+  <si>
+    <t>1713 REI DO HAMBURGUER LTDA</t>
+  </si>
+  <si>
+    <t>35.096.503/0001-97</t>
+  </si>
+  <si>
+    <t>LOJA FEIRÃO DA MODA, BKN 28149, MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>patriciasatyrofinanceiro@feiraomodario.net.br</t>
+  </si>
+  <si>
+    <t>012467</t>
+  </si>
+  <si>
+    <t>1710 INFO BURGER COMERCIO DE ALIMENTOS UNIPESSOAL LTDA</t>
+  </si>
+  <si>
+    <t>35.062.517/0001-90</t>
+  </si>
+  <si>
+    <t>EXTRA EUSÉBIO BKN 27591-  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>tatielebarroso@infoxparticipacoes.com</t>
+  </si>
+  <si>
+    <t>012468</t>
+  </si>
+  <si>
+    <t>1650 ARQUIDUQUE ALVIM COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>35.254.858/0001-67</t>
+  </si>
+  <si>
+    <t>LOJA SHOP PIER 21 BKN 21274  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>adm@grupoalvim.com.br</t>
+  </si>
+  <si>
+    <t>012469</t>
+  </si>
+  <si>
+    <t>1651 ESCUDEIRO ALVIM COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>35.252.660/0001-44</t>
+  </si>
+  <si>
+    <t>LOJA CARREFOUR BRASILIA SUL BKN 20212 -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012470</t>
+  </si>
+  <si>
+    <t>1657 CAVALEIRO ALVIM COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>35.378.393/0001-56</t>
+  </si>
+  <si>
+    <t>LOJA SHOP VENÂNCIO BKN 25261-MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012471</t>
+  </si>
+  <si>
+    <t>1648 SENHOR ALVIM COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>35.257.416/0001-74</t>
+  </si>
+  <si>
+    <t>LOJA IGUATEMI BRAS, BKN 23464  - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012472</t>
+  </si>
+  <si>
+    <t>1595 BARAO ALVIM COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>34.840.241/0001-60</t>
+  </si>
+  <si>
+    <t>LOJA PLANALTINA, BKN 27984 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012473</t>
+  </si>
+  <si>
+    <t>1649 REGENTE ALVIM COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>35.238.002/0001-06</t>
+  </si>
+  <si>
+    <t>ILR BRASÍLIA - ASA NORTE 201, BKN 19929 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012474</t>
+  </si>
+  <si>
+    <t>1658 VISCONDE COMERCIO DE ALIMENTOS LTDA ME</t>
+  </si>
+  <si>
+    <t>35.359.111/0001-73</t>
+  </si>
+  <si>
+    <t>LOJA CENTURY PLAZA BKN 21583 MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012475</t>
+  </si>
+  <si>
+    <t>1220 VILLE ALIMENTOS EIRELI</t>
+  </si>
+  <si>
+    <t>29.217.358/0002-33</t>
+  </si>
+  <si>
+    <t>KSK ESTAÇÃO DA LAPA  -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>cs.sampaio91@hotmail.com</t>
+  </si>
+  <si>
+    <t>012476</t>
+  </si>
+  <si>
+    <t>1221 VILLE ALIMENTOS EIRELI - EPP</t>
+  </si>
+  <si>
+    <t>29.217.358/0001-52</t>
+  </si>
+  <si>
+    <t>SHOPPING PIEDADE, BKN 25191- MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012477</t>
+  </si>
+  <si>
+    <t>1712 JDF NORDESTE EMPREENDIMENTO ALIMENTICIO LTDA</t>
+  </si>
+  <si>
+    <t>17.729.812/0003-37</t>
+  </si>
+  <si>
+    <t>BKN 28350 -LOJA SERRA TALHADA  - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>jdfjodibe@jodibe.com.br</t>
+  </si>
+  <si>
+    <t>012478</t>
+  </si>
+  <si>
+    <t>1711 B &amp; B HAMBURGUERIA LTDA</t>
+  </si>
+  <si>
+    <t>35.063.036/0001-07</t>
+  </si>
+  <si>
+    <t>BKN 28289 - LOJA ARAPONGAS, MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>beatriz@grupobeb.com</t>
+  </si>
+  <si>
+    <t>012479</t>
+  </si>
+  <si>
+    <t>1703 JIKALBK LANCHES LTDA</t>
+  </si>
+  <si>
+    <t>35.836.047/0001-74</t>
+  </si>
+  <si>
+    <t>LOJA K TOWN, BKN 28297- MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>contas@jikalbk.com.br</t>
+  </si>
+  <si>
+    <t>012480</t>
+  </si>
+  <si>
+    <t>1116 GAMA HAMBURGUER REI LTDA</t>
+  </si>
+  <si>
+    <t>28.128.788/0001-35</t>
+  </si>
+  <si>
+    <t>GAMA -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO** Reajuste aniversário do contrato - Índice IPCA 4,608220 % (acumulado 12 meses,  período de 09/22 até 08/23).</t>
+  </si>
+  <si>
+    <t>financeirobk12@gmail.com</t>
+  </si>
+  <si>
+    <t>012481</t>
+  </si>
+  <si>
+    <t>1117 HAMBURGUER REI LTDA</t>
+  </si>
+  <si>
+    <t>28.802.355/0001-13</t>
+  </si>
+  <si>
+    <t>GAMA ESTÁDIO -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012482</t>
+  </si>
+  <si>
+    <t>1061 BVS ALIMENTOS E CONGÊNERES EIRELI</t>
+  </si>
+  <si>
+    <t>31.856.290/0001-01</t>
+  </si>
+  <si>
+    <t>LOJA BUENA VISTA - BKN 26588 -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>guilhermeqc@terra.com.br</t>
+  </si>
+  <si>
+    <t>012483</t>
+  </si>
+  <si>
+    <t>1140 HG6 FOODS COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>29.203.250/0001-00</t>
+  </si>
+  <si>
+    <t>LOJA ACLIMAÇÃO -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>nataliako@casabueno.com.br</t>
+  </si>
+  <si>
+    <t>012484</t>
+  </si>
+  <si>
+    <t>1141 HG6 FOODS COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>29.203.250/0002-91</t>
+  </si>
+  <si>
+    <t>BK POMPÉIA  -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012485</t>
+  </si>
+  <si>
+    <t>1149 JHR SERVICOS DE ALIMENTACAO LTDA - EPP </t>
+  </si>
+  <si>
+    <t>26.995.025/0001-66</t>
+  </si>
+  <si>
+    <t>VIA VERDE  SHOPPING -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>daf@grupoaguanaboca.com</t>
+  </si>
+  <si>
+    <t>012486</t>
+  </si>
+  <si>
+    <t>1852 SAINT HONORE COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>26.716.832/0008-79</t>
+  </si>
+  <si>
+    <t>LOJA TOLEDO, BKN 29286 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>luciane@sthonore.com.br</t>
+  </si>
+  <si>
+    <t>012487</t>
+  </si>
+  <si>
+    <t>1059 OLIMPIA FAST FOOD LTDA</t>
+  </si>
+  <si>
+    <t>31.248.938/0001-59</t>
+  </si>
+  <si>
+    <t>LOJA OLÍMPIA MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>financeiro03.olimpiapark@enjoyhoteis.com.br</t>
+  </si>
+  <si>
+    <t>012488</t>
+  </si>
+  <si>
+    <t>1060 BURGER KING RIVER SHOPPING EIRELI - ME</t>
+  </si>
+  <si>
+    <t>28.036.959/0001-04</t>
+  </si>
+  <si>
+    <t>RIVER - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>campus.10@hotmail.com</t>
+  </si>
+  <si>
+    <t>012489</t>
+  </si>
+  <si>
+    <t>1062 CBA COMERCIO DE ALIMENTOS LTDA - ME </t>
+  </si>
+  <si>
+    <t>26.222.495/0001-97</t>
+  </si>
+  <si>
+    <t>JUÁ GARDEN SHOPPING MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012490</t>
+  </si>
+  <si>
+    <t>1064 CONDE ALVIM COMERCIO DE ALIMENTOS LTDA - ME</t>
+  </si>
+  <si>
+    <t>28.993.561/0001-58</t>
+  </si>
+  <si>
+    <t>AGUAS CLARAS MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012491</t>
+  </si>
+  <si>
+    <t>1066 CONFORTI COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>26.390.660/0004-62</t>
+  </si>
+  <si>
+    <t>LOJA MASCARENHAS MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012492</t>
+  </si>
+  <si>
+    <t>1067 CONFORTI COMERCIO DE ALIMENTOS LTDA </t>
+  </si>
+  <si>
+    <t>26.390.660/0003-81</t>
+  </si>
+  <si>
+    <t>LOJA NSUL -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012493</t>
+  </si>
+  <si>
+    <t>1068 CONFORTI COMERCIO DE ALIMENTOS LTDA </t>
+  </si>
+  <si>
+    <t>26.390.660/0001-10</t>
+  </si>
+  <si>
+    <t>LOJA PENA - MMENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012494</t>
+  </si>
+  <si>
+    <t>1069 CONFORTI COMERCIO DE ALIMENTOS LTDA </t>
+  </si>
+  <si>
+    <t>26.390.660/0002-09</t>
+  </si>
+  <si>
+    <t>LOJA BOSQUE - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012495</t>
+  </si>
+  <si>
+    <t>1093 DUQUE ALVIM COMERCIO DE ALIMENTOS LTDA - ME</t>
+  </si>
+  <si>
+    <t>29.087.671/0001-13</t>
+  </si>
+  <si>
+    <t>LAGO SUL MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012496</t>
+  </si>
+  <si>
+    <t>1094 E. A. Dos SANTOS SOUSA EIRELI - ME</t>
+  </si>
+  <si>
+    <t>24.668.421/0001-53</t>
+  </si>
+  <si>
+    <t>PARAUPEBAS - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>financeiro.bkmab@gmail.com</t>
+  </si>
+  <si>
+    <t>012497</t>
+  </si>
+  <si>
+    <t>1120 GLADIADOR ALVIM COMERCIO DE ALIMENTOS LTDA - ME </t>
+  </si>
+  <si>
+    <t>28.953.109/0001-62</t>
+  </si>
+  <si>
+    <t>ASA SUL - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012498</t>
+  </si>
+  <si>
+    <t>1139 HF MOTA ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>31.006.458/0001-81</t>
+  </si>
+  <si>
+    <t>LOJA ÔNIX  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>mota@hfmota.com.br</t>
+  </si>
+  <si>
+    <t>012499</t>
+  </si>
+  <si>
+    <t>1142 IMPERADOR ALVIM COMERCIO DE ALIMENTOS LTDA - ME </t>
+  </si>
+  <si>
+    <t>26.428.809/0001-02</t>
+  </si>
+  <si>
+    <t>ASA NORTE MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012500</t>
+  </si>
+  <si>
+    <t>1166 LKL COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>29.830.339/0001-05</t>
+  </si>
+  <si>
+    <t>BK CARIRI  -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>burgerkingcariri@hotmail.com</t>
+  </si>
+  <si>
+    <t>012501</t>
+  </si>
+  <si>
+    <t>1167 LORD ALVIM COMERCIO DE ALIMENTOS LTDA </t>
+  </si>
+  <si>
+    <t>26.332.112/0001-33</t>
+  </si>
+  <si>
+    <t>SUDOESTE BRASILIA MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012502</t>
+  </si>
+  <si>
+    <t>1168 M E A DOS SANTOS SANTOS EIRELI - EPP</t>
+  </si>
+  <si>
+    <t>28.440.986/0001-30</t>
+  </si>
+  <si>
+    <t>PATIO MARABA MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012503</t>
+  </si>
+  <si>
+    <t>1173 MOREIRA &amp; AZEVEDO COMERCIAL LTDA - EPP</t>
+  </si>
+  <si>
+    <t>29.264.680/0001-32</t>
+  </si>
+  <si>
+    <t>PATIO MIX BAHIA - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>cdagf@hotmail.com</t>
+  </si>
+  <si>
+    <t>012504</t>
+  </si>
+  <si>
+    <t>1180 PAMPA RESTAURANTES LTDA</t>
+  </si>
+  <si>
+    <t>27.451.986/0006-87</t>
+  </si>
+  <si>
+    <t>FORT ATACADISTA - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>bk.financeiro@pampa.net</t>
+  </si>
+  <si>
+    <t>012505</t>
+  </si>
+  <si>
+    <t>1181 PAMPA RESTAURANTES LTDA - EPP</t>
+  </si>
+  <si>
+    <t>27.451.986/0009-20</t>
+  </si>
+  <si>
+    <t>CACOAL MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012506</t>
+  </si>
+  <si>
+    <t>1183 PAMPA RESTAURANTES LTDA - EPP</t>
+  </si>
+  <si>
+    <t>27.451.986/0004-15</t>
+  </si>
+  <si>
+    <t>LOJA  TANGARÁ DA SERRA MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012507</t>
+  </si>
+  <si>
+    <t>1184 PAMPA RESTAURANTES LTDA - EPP</t>
+  </si>
+  <si>
+    <t>27.451.986/0005-04</t>
+  </si>
+  <si>
+    <t>LOJA GABRIELA MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012508</t>
+  </si>
+  <si>
+    <t>1185 PAMPA RESTAURANTES LTDA - EPP </t>
+  </si>
+  <si>
+    <t>27.451.986/0002-53</t>
+  </si>
+  <si>
+    <t>PORTO VELHO MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012509</t>
+  </si>
+  <si>
+    <t>1186 PAMPA RESTAURANTES LTDA - EPP </t>
+  </si>
+  <si>
+    <t>27.451.986/0003-34</t>
+  </si>
+  <si>
+    <t>LOJA QUIOSQUE - SUPERMERCADO COMPER  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012510</t>
+  </si>
+  <si>
+    <t>1188 PAMPA RESTAURANTES LTDA - EPP </t>
+  </si>
+  <si>
+    <t>27.451.986/0010-63</t>
+  </si>
+  <si>
+    <t>JI PARANA - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012511</t>
+  </si>
+  <si>
+    <t>1189 PRINCE COMERCIO DE ALIMENTOS EIRELI - EPP</t>
+  </si>
+  <si>
+    <t>28.028.490/0001-53</t>
+  </si>
+  <si>
+    <t>SPIPE CALARGE  - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012512</t>
+  </si>
+  <si>
+    <t>1190 PRINCIPE ALVIM COMERCIO DE ALIMENTOS EIRELI - ME</t>
+  </si>
+  <si>
+    <t>28.428.268/0001-48</t>
+  </si>
+  <si>
+    <t>CEILANDIA - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012513</t>
+  </si>
+  <si>
+    <t>1193 RCMI ALIMENTACAO LTDA - EPP </t>
+  </si>
+  <si>
+    <t>27.928.572/0001-91</t>
+  </si>
+  <si>
+    <t>UBERLANDIA  -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012514</t>
+  </si>
+  <si>
+    <t>1194 REI ALVIM COMERCIO DE ALIMENTOS EIRELI </t>
+  </si>
+  <si>
+    <t>26.075.154/0001-36</t>
+  </si>
+  <si>
+    <t>CALDAS NOVAS SHOPPING  - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
+  </si>
+  <si>
+    <t>012515</t>
+  </si>
+  <si>
+    <t>1196 RMF FAST FOODS EIRELI</t>
+  </si>
+  <si>
+    <t>20.255.764/0007-20</t>
+  </si>
+  <si>
+    <t>ILHÉUS CENTRO  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS  REF SETEMBRO</t>
+  </si>
+  <si>
     <t>paulo.vieira@grupormfba.com.br</t>
-  </si>
-  <si>
-    <t>012459</t>
-  </si>
-  <si>
-    <t>1673 CAMPOS CHAVES PRODUTOS ALIMENTICIOS LTDA</t>
-  </si>
-  <si>
-    <t>34.798.861/0001-89</t>
-  </si>
-  <si>
-    <t>LOJA GOVERNADOR VALADARES, BKN 27996 -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>setorfinanceiro.uniao@gmail.com</t>
-  </si>
-  <si>
-    <t>012460</t>
-  </si>
-  <si>
-    <t>1659 CONFORTI COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>26.390.660/0006-24</t>
-  </si>
-  <si>
-    <t>LOJA CAMPO GRANDE - MT  BKN 27986 -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>financeiro@bkconforti.com</t>
-  </si>
-  <si>
-    <t>012461</t>
-  </si>
-  <si>
-    <t>1665 RCPM ALIMENTACAO LTDA</t>
-  </si>
-  <si>
-    <t>34.854.503/0001-46</t>
-  </si>
-  <si>
-    <t>LOJA OIAPOQUE BKN 25048 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>ricardo.de.campos@hotmail.com</t>
-  </si>
-  <si>
-    <t>012462</t>
-  </si>
-  <si>
-    <t>1597 BK BLESS COMERCIO DE ALIMENTOS EIRELI</t>
-  </si>
-  <si>
-    <t>34.911.443/0003-18</t>
-  </si>
-  <si>
-    <t>LOJA ZAFFARI HÍPICA BKN 27993- MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>financeiro.bk@empresasbless.com.br</t>
-  </si>
-  <si>
-    <t>012463</t>
-  </si>
-  <si>
-    <t>1667 BK BLESS COMERCIO DE ALIMENTOS EIRELI</t>
-  </si>
-  <si>
-    <t>34.911.443/0002-37</t>
-  </si>
-  <si>
-    <t>LOJA JOÃO PESSOA SHOPPING BKN 27992 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012464</t>
-  </si>
-  <si>
-    <t>1686 3A LANCHONETE LTDA</t>
-  </si>
-  <si>
-    <t>34.953.955/0001-85</t>
-  </si>
-  <si>
-    <t>ALPHA SHOPPING BKN 27592 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>alphashopping.bk@gmail.com</t>
-  </si>
-  <si>
-    <t>012465</t>
-  </si>
-  <si>
-    <t>1676 ELM COMÉRCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>35.561.003/0001-89</t>
-  </si>
-  <si>
-    <t>LOJA GREEN PLAZA - MG  BKN 28227 MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>bkgreenplaza@gmail.com</t>
-  </si>
-  <si>
-    <t>012466</t>
-  </si>
-  <si>
-    <t>1713 REI DO HAMBURGUER LTDA</t>
-  </si>
-  <si>
-    <t>35.096.503/0001-97</t>
-  </si>
-  <si>
-    <t>LOJA FEIRÃO DA MODA, BKN 28149, MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>patriciasatyrofinanceiro@feiraomodario.net.br</t>
-  </si>
-  <si>
-    <t>012467</t>
-  </si>
-  <si>
-    <t>1710 INFO BURGER COMERCIO DE ALIMENTOS UNIPESSOAL LTDA</t>
-  </si>
-  <si>
-    <t>35.062.517/0001-90</t>
-  </si>
-  <si>
-    <t>EXTRA EUSÉBIO BKN 27591-  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>tatielebarroso@infoxparticipacoes.com</t>
-  </si>
-  <si>
-    <t>012468</t>
-  </si>
-  <si>
-    <t>1650 ARQUIDUQUE ALVIM COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>35.254.858/0001-67</t>
-  </si>
-  <si>
-    <t>LOJA SHOP PIER 21 BKN 21274  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>adm@grupoalvim.com.br</t>
-  </si>
-  <si>
-    <t>012469</t>
-  </si>
-  <si>
-    <t>1651 ESCUDEIRO ALVIM COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>35.252.660/0001-44</t>
-  </si>
-  <si>
-    <t>LOJA CARREFOUR BRASILIA SUL BKN 20212 -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012470</t>
-  </si>
-  <si>
-    <t>1657 CAVALEIRO ALVIM COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>35.378.393/0001-56</t>
-  </si>
-  <si>
-    <t>LOJA SHOP VENÂNCIO BKN 25261-MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012471</t>
-  </si>
-  <si>
-    <t>1648 SENHOR ALVIM COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>35.257.416/0001-74</t>
-  </si>
-  <si>
-    <t>LOJA IGUATEMI BRAS, BKN 23464  - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012472</t>
-  </si>
-  <si>
-    <t>1595 BARAO ALVIM COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>34.840.241/0001-60</t>
-  </si>
-  <si>
-    <t>LOJA PLANALTINA, BKN 27984 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012473</t>
-  </si>
-  <si>
-    <t>1649 REGENTE ALVIM COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>35.238.002/0001-06</t>
-  </si>
-  <si>
-    <t>ILR BRASÍLIA - ASA NORTE 201, BKN 19929 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012474</t>
-  </si>
-  <si>
-    <t>1658 VISCONDE COMERCIO DE ALIMENTOS LTDA ME</t>
-  </si>
-  <si>
-    <t>35.359.111/0001-73</t>
-  </si>
-  <si>
-    <t>LOJA CENTURY PLAZA BKN 21583 MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012475</t>
-  </si>
-  <si>
-    <t>1220 VILLE ALIMENTOS EIRELI</t>
-  </si>
-  <si>
-    <t>29.217.358/0002-33</t>
-  </si>
-  <si>
-    <t>KSK ESTAÇÃO DA LAPA  -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>cs.sampaio91@hotmail.com</t>
-  </si>
-  <si>
-    <t>012476</t>
-  </si>
-  <si>
-    <t>1221 VILLE ALIMENTOS EIRELI - EPP</t>
-  </si>
-  <si>
-    <t>29.217.358/0001-52</t>
-  </si>
-  <si>
-    <t>SHOPPING PIEDADE, BKN 25191- MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012477</t>
-  </si>
-  <si>
-    <t>1712 JDF NORDESTE EMPREENDIMENTO ALIMENTICIO LTDA</t>
-  </si>
-  <si>
-    <t>17.729.812/0003-37</t>
-  </si>
-  <si>
-    <t>BKN 28350 -LOJA SERRA TALHADA  - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>jdfjodibe@jodibe.com.br</t>
-  </si>
-  <si>
-    <t>012478</t>
-  </si>
-  <si>
-    <t>1711 B &amp; B HAMBURGUERIA LTDA</t>
-  </si>
-  <si>
-    <t>35.063.036/0001-07</t>
-  </si>
-  <si>
-    <t>BKN 28289 - LOJA ARAPONGAS, MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>beatriz@grupobeb.com</t>
-  </si>
-  <si>
-    <t>012479</t>
-  </si>
-  <si>
-    <t>1703 JIKALBK LANCHES LTDA</t>
-  </si>
-  <si>
-    <t>35.836.047/0001-74</t>
-  </si>
-  <si>
-    <t>LOJA K TOWN, BKN 28297- MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>contas@jikalbk.com.br</t>
-  </si>
-  <si>
-    <t>012480</t>
-  </si>
-  <si>
-    <t>1116 GAMA HAMBURGUER REI LTDA</t>
-  </si>
-  <si>
-    <t>28.128.788/0001-35</t>
-  </si>
-  <si>
-    <t>GAMA -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO** Reajuste aniversário do contrato - Índice IPCA 4,608220 % (acumulado 12 meses,  período de 09/22 até 08/23).</t>
-  </si>
-  <si>
-    <t>financeirobk12@gmail.com</t>
-  </si>
-  <si>
-    <t>012481</t>
-  </si>
-  <si>
-    <t>1117 HAMBURGUER REI LTDA</t>
-  </si>
-  <si>
-    <t>28.802.355/0001-13</t>
-  </si>
-  <si>
-    <t>GAMA ESTÁDIO -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012482</t>
-  </si>
-  <si>
-    <t>1061 BVS ALIMENTOS E CONGÊNERES EIRELI</t>
-  </si>
-  <si>
-    <t>31.856.290/0001-01</t>
-  </si>
-  <si>
-    <t>LOJA BUENA VISTA - BKN 26588 -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>guilhermeqc@terra.com.br</t>
-  </si>
-  <si>
-    <t>012483</t>
-  </si>
-  <si>
-    <t>1140 HG6 FOODS COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>29.203.250/0001-00</t>
-  </si>
-  <si>
-    <t>LOJA ACLIMAÇÃO -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>nataliako@casabueno.com.br</t>
-  </si>
-  <si>
-    <t>012484</t>
-  </si>
-  <si>
-    <t>1141 HG6 FOODS COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>29.203.250/0002-91</t>
-  </si>
-  <si>
-    <t>BK POMPÉIA  -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012485</t>
-  </si>
-  <si>
-    <t>1149 JHR SERVICOS DE ALIMENTACAO LTDA - EPP </t>
-  </si>
-  <si>
-    <t>26.995.025/0001-66</t>
-  </si>
-  <si>
-    <t>VIA VERDE  SHOPPING -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>daf@grupoaguanaboca.com</t>
-  </si>
-  <si>
-    <t>012486</t>
-  </si>
-  <si>
-    <t>1852 SAINT HONORE COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>26.716.832/0008-79</t>
-  </si>
-  <si>
-    <t>LOJA TOLEDO, BKN 29286 - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>luciane@sthonore.com.br</t>
-  </si>
-  <si>
-    <t>012487</t>
-  </si>
-  <si>
-    <t>1059 OLIMPIA FAST FOOD LTDA</t>
-  </si>
-  <si>
-    <t>31.248.938/0001-59</t>
-  </si>
-  <si>
-    <t>LOJA OLÍMPIA MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>financeiro03.olimpiapark@enjoyhoteis.com.br</t>
-  </si>
-  <si>
-    <t>012488</t>
-  </si>
-  <si>
-    <t>1060 BURGER KING RIVER SHOPPING EIRELI - ME</t>
-  </si>
-  <si>
-    <t>28.036.959/0001-04</t>
-  </si>
-  <si>
-    <t>RIVER - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>campus.10@hotmail.com</t>
-  </si>
-  <si>
-    <t>012489</t>
-  </si>
-  <si>
-    <t>1062 CBA COMERCIO DE ALIMENTOS LTDA - ME </t>
-  </si>
-  <si>
-    <t>26.222.495/0001-97</t>
-  </si>
-  <si>
-    <t>JUÁ GARDEN SHOPPING MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012490</t>
-  </si>
-  <si>
-    <t>1064 CONDE ALVIM COMERCIO DE ALIMENTOS LTDA - ME</t>
-  </si>
-  <si>
-    <t>28.993.561/0001-58</t>
-  </si>
-  <si>
-    <t>AGUAS CLARAS MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012491</t>
-  </si>
-  <si>
-    <t>1066 CONFORTI COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>26.390.660/0004-62</t>
-  </si>
-  <si>
-    <t>LOJA MASCARENHAS MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012492</t>
-  </si>
-  <si>
-    <t>1067 CONFORTI COMERCIO DE ALIMENTOS LTDA </t>
-  </si>
-  <si>
-    <t>26.390.660/0003-81</t>
-  </si>
-  <si>
-    <t>LOJA NSUL -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012493</t>
-  </si>
-  <si>
-    <t>1068 CONFORTI COMERCIO DE ALIMENTOS LTDA </t>
-  </si>
-  <si>
-    <t>26.390.660/0001-10</t>
-  </si>
-  <si>
-    <t>LOJA PENA - MMENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012494</t>
-  </si>
-  <si>
-    <t>1069 CONFORTI COMERCIO DE ALIMENTOS LTDA </t>
-  </si>
-  <si>
-    <t>26.390.660/0002-09</t>
-  </si>
-  <si>
-    <t>LOJA BOSQUE - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012495</t>
-  </si>
-  <si>
-    <t>1093 DUQUE ALVIM COMERCIO DE ALIMENTOS LTDA - ME</t>
-  </si>
-  <si>
-    <t>29.087.671/0001-13</t>
-  </si>
-  <si>
-    <t>LAGO SUL MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012496</t>
-  </si>
-  <si>
-    <t>1094 E. A. Dos SANTOS SOUSA EIRELI - ME</t>
-  </si>
-  <si>
-    <t>24.668.421/0001-53</t>
-  </si>
-  <si>
-    <t>PARAUPEBAS - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>financeiro.bkmab@gmail.com</t>
-  </si>
-  <si>
-    <t>012497</t>
-  </si>
-  <si>
-    <t>1120 GLADIADOR ALVIM COMERCIO DE ALIMENTOS LTDA - ME </t>
-  </si>
-  <si>
-    <t>28.953.109/0001-62</t>
-  </si>
-  <si>
-    <t>ASA SUL - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012498</t>
-  </si>
-  <si>
-    <t>1139 HF MOTA ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>31.006.458/0001-81</t>
-  </si>
-  <si>
-    <t>LOJA ÔNIX  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>mota@hfmota.com.br</t>
-  </si>
-  <si>
-    <t>012499</t>
-  </si>
-  <si>
-    <t>1142 IMPERADOR ALVIM COMERCIO DE ALIMENTOS LTDA - ME </t>
-  </si>
-  <si>
-    <t>26.428.809/0001-02</t>
-  </si>
-  <si>
-    <t>ASA NORTE MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012500</t>
-  </si>
-  <si>
-    <t>1166 LKL COMERCIO DE ALIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>29.830.339/0001-05</t>
-  </si>
-  <si>
-    <t>BK CARIRI  -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>burgerkingcariri@hotmail.com</t>
-  </si>
-  <si>
-    <t>012501</t>
-  </si>
-  <si>
-    <t>1167 LORD ALVIM COMERCIO DE ALIMENTOS LTDA </t>
-  </si>
-  <si>
-    <t>26.332.112/0001-33</t>
-  </si>
-  <si>
-    <t>SUDOESTE BRASILIA MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012502</t>
-  </si>
-  <si>
-    <t>1168 M E A DOS SANTOS SANTOS EIRELI - EPP</t>
-  </si>
-  <si>
-    <t>28.440.986/0001-30</t>
-  </si>
-  <si>
-    <t>PATIO MARABA MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012503</t>
-  </si>
-  <si>
-    <t>1173 MOREIRA &amp; AZEVEDO COMERCIAL LTDA - EPP</t>
-  </si>
-  <si>
-    <t>29.264.680/0001-32</t>
-  </si>
-  <si>
-    <t>PATIO MIX BAHIA - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>cdagf@hotmail.com</t>
-  </si>
-  <si>
-    <t>012504</t>
-  </si>
-  <si>
-    <t>1180 PAMPA RESTAURANTES LTDA</t>
-  </si>
-  <si>
-    <t>27.451.986/0006-87</t>
-  </si>
-  <si>
-    <t>FORT ATACADISTA - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>bk.financeiro@pampa.net</t>
-  </si>
-  <si>
-    <t>012505</t>
-  </si>
-  <si>
-    <t>1181 PAMPA RESTAURANTES LTDA - EPP</t>
-  </si>
-  <si>
-    <t>27.451.986/0009-20</t>
-  </si>
-  <si>
-    <t>CACOAL MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012506</t>
-  </si>
-  <si>
-    <t>1183 PAMPA RESTAURANTES LTDA - EPP</t>
-  </si>
-  <si>
-    <t>27.451.986/0004-15</t>
-  </si>
-  <si>
-    <t>LOJA  TANGARÁ DA SERRA MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012507</t>
-  </si>
-  <si>
-    <t>1184 PAMPA RESTAURANTES LTDA - EPP</t>
-  </si>
-  <si>
-    <t>27.451.986/0005-04</t>
-  </si>
-  <si>
-    <t>LOJA GABRIELA MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012508</t>
-  </si>
-  <si>
-    <t>1185 PAMPA RESTAURANTES LTDA - EPP </t>
-  </si>
-  <si>
-    <t>27.451.986/0002-53</t>
-  </si>
-  <si>
-    <t>PORTO VELHO MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012509</t>
-  </si>
-  <si>
-    <t>1186 PAMPA RESTAURANTES LTDA - EPP </t>
-  </si>
-  <si>
-    <t>27.451.986/0003-34</t>
-  </si>
-  <si>
-    <t>LOJA QUIOSQUE - SUPERMERCADO COMPER  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012510</t>
-  </si>
-  <si>
-    <t>1188 PAMPA RESTAURANTES LTDA - EPP </t>
-  </si>
-  <si>
-    <t>27.451.986/0010-63</t>
-  </si>
-  <si>
-    <t>JI PARANA - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012511</t>
-  </si>
-  <si>
-    <t>1189 PRINCE COMERCIO DE ALIMENTOS EIRELI - EPP</t>
-  </si>
-  <si>
-    <t>28.028.490/0001-53</t>
-  </si>
-  <si>
-    <t>SPIPE CALARGE  - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012512</t>
-  </si>
-  <si>
-    <t>1190 PRINCIPE ALVIM COMERCIO DE ALIMENTOS EIRELI - ME</t>
-  </si>
-  <si>
-    <t>28.428.268/0001-48</t>
-  </si>
-  <si>
-    <t>CEILANDIA - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012513</t>
-  </si>
-  <si>
-    <t>1193 RCMI ALIMENTACAO LTDA - EPP </t>
-  </si>
-  <si>
-    <t>27.928.572/0001-91</t>
-  </si>
-  <si>
-    <t>UBERLANDIA  -  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012514</t>
-  </si>
-  <si>
-    <t>1194 REI ALVIM COMERCIO DE ALIMENTOS EIRELI </t>
-  </si>
-  <si>
-    <t>26.075.154/0001-36</t>
-  </si>
-  <si>
-    <t>CALDAS NOVAS SHOPPING  - MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS REF SETEMBRO</t>
-  </si>
-  <si>
-    <t>012515</t>
-  </si>
-  <si>
-    <t>1196 RMF FAST FOODS EIRELI</t>
-  </si>
-  <si>
-    <t>20.255.764/0007-20</t>
-  </si>
-  <si>
-    <t>ILHÉUS CENTRO  MENSALIDADES SUPORTES N1 POS + DIGITAL, POS + N3, SERVIÇO DE ATUALIZAÇÃO DE PREÇOS  REF SETEMBRO</t>
   </si>
   <si>
     <t>012516</t>
@@ -1080,7 +1074,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1239,6 +1233,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1590,7 +1590,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1599,6 +1599,7 @@
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
     <xf numFmtId="40" fontId="20" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1959,7 +1960,7 @@
   <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2149,7 +2150,7 @@
         <v>45236</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2166,13 +2167,13 @@
         <v>12452</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="H6" s="4">
         <v>644.74</v>
@@ -2184,7 +2185,7 @@
         <v>45236</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2198,16 +2199,16 @@
         <v>45210</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="H7" s="4">
         <v>688.64</v>
@@ -2219,7 +2220,7 @@
         <v>45245</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2233,16 +2234,16 @@
         <v>45210</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="H8" s="4">
         <v>684.27</v>
@@ -2254,7 +2255,7 @@
         <v>45236</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2268,16 +2269,16 @@
         <v>45210</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="H9" s="4">
         <v>651.22</v>
@@ -2288,8 +2289,8 @@
       <c r="J9" s="3">
         <v>45236</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>43</v>
+      <c r="K9" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2303,16 +2304,16 @@
         <v>45210</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="H10" s="4">
         <v>637.12</v>
@@ -2323,8 +2324,8 @@
       <c r="J10" s="3">
         <v>45240</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>48</v>
+      <c r="K10" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2338,16 +2339,16 @@
         <v>45210</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="H11" s="4">
         <v>636.41999999999996</v>
@@ -2358,8 +2359,8 @@
       <c r="J11" s="3">
         <v>45240</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>48</v>
+      <c r="K11" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2373,16 +2374,16 @@
         <v>45210</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="H12" s="4">
         <v>637.12</v>
@@ -2393,8 +2394,8 @@
       <c r="J12" s="3">
         <v>45236</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>57</v>
+      <c r="K12" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2408,16 +2409,16 @@
         <v>45210</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="H13" s="4">
         <v>637.12</v>
@@ -2429,7 +2430,7 @@
         <v>45236</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2443,16 +2444,16 @@
         <v>45210</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H14" s="4">
         <v>637.12</v>
@@ -2464,7 +2465,7 @@
         <v>45236</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2478,16 +2479,16 @@
         <v>45210</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="H15" s="4">
         <v>651.22</v>
@@ -2499,7 +2500,7 @@
         <v>45236</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2513,16 +2514,16 @@
         <v>45210</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="H16" s="4">
         <v>637.12</v>
@@ -2534,7 +2535,7 @@
         <v>45236</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2548,16 +2549,16 @@
         <v>45210</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="H17" s="4">
         <v>601.62</v>
@@ -2569,7 +2570,7 @@
         <v>45236</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2583,16 +2584,16 @@
         <v>45210</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="H18" s="4">
         <v>637.12</v>
@@ -2604,7 +2605,7 @@
         <v>45236</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -2618,16 +2619,16 @@
         <v>45210</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="H19" s="4">
         <v>637.12</v>
@@ -2639,7 +2640,7 @@
         <v>45236</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -2653,16 +2654,16 @@
         <v>45210</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="H20" s="4">
         <v>636.29999999999995</v>
@@ -2674,7 +2675,7 @@
         <v>45236</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2688,16 +2689,16 @@
         <v>45210</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="H21" s="4">
         <v>651.22</v>
@@ -2709,7 +2710,7 @@
         <v>45236</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -2723,16 +2724,16 @@
         <v>45210</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="H22" s="4">
         <v>651.22</v>
@@ -2744,7 +2745,7 @@
         <v>45236</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2758,16 +2759,16 @@
         <v>45210</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="H23" s="4">
         <v>651.22</v>
@@ -2779,7 +2780,7 @@
         <v>45236</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -2793,16 +2794,16 @@
         <v>45210</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="H24" s="4">
         <v>651.22</v>
@@ -2814,7 +2815,7 @@
         <v>45236</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2828,16 +2829,16 @@
         <v>45210</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="H25" s="4">
         <v>651.22</v>
@@ -2849,7 +2850,7 @@
         <v>45236</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2863,16 +2864,16 @@
         <v>45210</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="H26" s="4">
         <v>637.12</v>
@@ -2884,7 +2885,7 @@
         <v>45236</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2898,16 +2899,16 @@
         <v>45210</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="H27" s="4">
         <v>637.12</v>
@@ -2919,7 +2920,7 @@
         <v>45236</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2933,16 +2934,16 @@
         <v>45210</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="H28" s="4">
         <v>651.22</v>
@@ -2954,7 +2955,7 @@
         <v>45236</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2968,16 +2969,16 @@
         <v>45210</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="H29" s="4">
         <v>370.66</v>
@@ -2989,7 +2990,7 @@
         <v>45245</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -3003,16 +3004,16 @@
         <v>45210</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="H30" s="4">
         <v>636.36</v>
@@ -3024,7 +3025,7 @@
         <v>45245</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -3038,16 +3039,16 @@
         <v>45210</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="H31" s="4">
         <v>688.64</v>
@@ -3059,7 +3060,7 @@
         <v>45236</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -3073,16 +3074,16 @@
         <v>45210</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="H32" s="4">
         <v>688.64</v>
@@ -3094,7 +3095,7 @@
         <v>45236</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -3108,16 +3109,16 @@
         <v>45210</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="H33" s="4">
         <v>694.42</v>
@@ -3129,7 +3130,7 @@
         <v>45236</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -3143,16 +3144,16 @@
         <v>45210</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="H34" s="4">
         <v>684.27</v>
@@ -3164,7 +3165,7 @@
         <v>45245</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -3178,16 +3179,16 @@
         <v>45210</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="H35" s="4">
         <v>637.12</v>
@@ -3199,7 +3200,7 @@
         <v>45245</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -3213,16 +3214,16 @@
         <v>45210</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="H36" s="4">
         <v>637.12</v>
@@ -3234,7 +3235,7 @@
         <v>45245</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -3248,16 +3249,16 @@
         <v>45210</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="H37" s="4">
         <v>637.12</v>
@@ -3269,7 +3270,7 @@
         <v>45236</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -3283,16 +3284,16 @@
         <v>45210</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="H38" s="4">
         <v>635.29999999999995</v>
@@ -3304,7 +3305,7 @@
         <v>45236</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -3318,16 +3319,16 @@
         <v>45210</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="H39" s="4">
         <v>629.6</v>
@@ -3339,7 +3340,7 @@
         <v>45236</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -3353,16 +3354,16 @@
         <v>45210</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="H40" s="4">
         <v>637.12</v>
@@ -3374,7 +3375,7 @@
         <v>45245</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -3388,16 +3389,16 @@
         <v>45210</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="H41" s="4">
         <v>601.62</v>
@@ -3409,7 +3410,7 @@
         <v>45236</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -3423,16 +3424,16 @@
         <v>45210</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="H42" s="4">
         <v>630.11</v>
@@ -3444,7 +3445,7 @@
         <v>45236</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -3458,16 +3459,16 @@
         <v>45210</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="H43" s="4">
         <v>651.22</v>
@@ -3479,7 +3480,7 @@
         <v>45236</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -3493,16 +3494,16 @@
         <v>45210</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="H44" s="4">
         <v>601.62</v>
@@ -3514,7 +3515,7 @@
         <v>45236</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -3528,16 +3529,16 @@
         <v>45210</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="H45" s="4">
         <v>630.11</v>
@@ -3549,7 +3550,7 @@
         <v>45236</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -3563,16 +3564,16 @@
         <v>45210</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="H46" s="4">
         <v>630.11</v>
@@ -3584,7 +3585,7 @@
         <v>45236</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -3598,16 +3599,16 @@
         <v>45210</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="H47" s="4">
         <v>637.12</v>
@@ -3619,7 +3620,7 @@
         <v>45236</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -3633,16 +3634,16 @@
         <v>45210</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="H48" s="4">
         <v>637.12</v>
@@ -3654,7 +3655,7 @@
         <v>45236</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -3668,16 +3669,16 @@
         <v>45210</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="H49" s="4">
         <v>637.12</v>
@@ -3689,7 +3690,7 @@
         <v>45236</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -3703,16 +3704,16 @@
         <v>45210</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="H50" s="4">
         <v>636.41999999999996</v>
@@ -3724,7 +3725,7 @@
         <v>45236</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -3738,16 +3739,16 @@
         <v>45210</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="H51" s="4">
         <v>651.22</v>
@@ -3759,7 +3760,7 @@
         <v>45236</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -3773,16 +3774,16 @@
         <v>45210</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="H52" s="4">
         <v>651.22</v>
@@ -3794,7 +3795,7 @@
         <v>45236</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -3808,16 +3809,16 @@
         <v>45210</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="H53" s="4">
         <v>636.41999999999996</v>
@@ -3829,7 +3830,7 @@
         <v>45236</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -3843,16 +3844,16 @@
         <v>45210</v>
       </c>
       <c r="D54" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="H54" s="4">
         <v>625.29999999999995</v>
@@ -3864,7 +3865,7 @@
         <v>45236</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -3878,16 +3879,16 @@
         <v>45210</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="H55" s="4">
         <v>636.41999999999996</v>
@@ -3899,7 +3900,7 @@
         <v>45236</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -3913,16 +3914,16 @@
         <v>45210</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="H56" s="4">
         <v>637.12</v>
@@ -3934,7 +3935,7 @@
         <v>45236</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -3948,16 +3949,16 @@
         <v>45210</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="H57" s="4">
         <v>637.12</v>
@@ -3969,7 +3970,7 @@
         <v>45236</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -3983,16 +3984,16 @@
         <v>45210</v>
       </c>
       <c r="D58" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="H58" s="4">
         <v>601.62</v>
@@ -4004,7 +4005,7 @@
         <v>45236</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -4018,16 +4019,16 @@
         <v>45210</v>
       </c>
       <c r="D59" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>270</v>
       </c>
       <c r="H59" s="4">
         <v>636.41999999999996</v>
@@ -4039,7 +4040,7 @@
         <v>45236</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -4053,16 +4054,16 @@
         <v>45210</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="H60" s="4">
         <v>637.12</v>
@@ -4074,7 +4075,7 @@
         <v>45236</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -4088,16 +4089,16 @@
         <v>45210</v>
       </c>
       <c r="D61" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="H61" s="4">
         <v>601.62</v>
@@ -4109,7 +4110,7 @@
         <v>45236</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -4123,16 +4124,16 @@
         <v>45210</v>
       </c>
       <c r="D62" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="H62" s="4">
         <v>644.74</v>
@@ -4144,7 +4145,7 @@
         <v>45236</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -4158,16 +4159,16 @@
         <v>45210</v>
       </c>
       <c r="D63" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="H63" s="4">
         <v>636.41999999999996</v>
@@ -4179,7 +4180,7 @@
         <v>45236</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -4193,16 +4194,16 @@
         <v>45210</v>
       </c>
       <c r="D64" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="H64" s="4">
         <v>636.41999999999996</v>
@@ -4214,7 +4215,7 @@
         <v>45236</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -4228,16 +4229,16 @@
         <v>45210</v>
       </c>
       <c r="D65" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="H65" s="4">
         <v>644.74</v>
@@ -4249,7 +4250,7 @@
         <v>45236</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -4263,16 +4264,16 @@
         <v>45210</v>
       </c>
       <c r="D66" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>298</v>
       </c>
       <c r="H66" s="4">
         <v>651.22</v>
@@ -4284,7 +4285,7 @@
         <v>45236</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -4298,16 +4299,16 @@
         <v>45210</v>
       </c>
       <c r="D67" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="H67" s="4">
         <v>644.74</v>
@@ -4319,7 +4320,7 @@
         <v>45236</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -4333,16 +4334,16 @@
         <v>45210</v>
       </c>
       <c r="D68" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>306</v>
       </c>
       <c r="H68" s="4">
         <v>688.64</v>
@@ -4354,7 +4355,7 @@
         <v>45236</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -4368,16 +4369,16 @@
         <v>45210</v>
       </c>
       <c r="D69" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G69" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="H69" s="4">
         <v>644.74</v>
@@ -4389,7 +4390,7 @@
         <v>45236</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>57</v>
+        <v>308</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -4403,16 +4404,16 @@
         <v>45210</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="H70" s="4">
         <v>626.79</v>
@@ -4424,7 +4425,7 @@
         <v>45236</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -4438,16 +4439,16 @@
         <v>45210</v>
       </c>
       <c r="D71" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F71" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="G71" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>319</v>
       </c>
       <c r="H71" s="4">
         <v>688.64</v>
@@ -4459,7 +4460,7 @@
         <v>45236</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -4473,16 +4474,16 @@
         <v>45210</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="G72" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="H72" s="4">
         <v>637.12</v>
@@ -4494,7 +4495,7 @@
         <v>45236</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -4508,16 +4509,16 @@
         <v>45210</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="G73" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>329</v>
       </c>
       <c r="H73" s="4">
         <v>684.27</v>
@@ -4529,7 +4530,7 @@
         <v>45236</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -4543,16 +4544,16 @@
         <v>45210</v>
       </c>
       <c r="D74" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F74" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="G74" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>334</v>
       </c>
       <c r="H74" s="4">
         <v>684.27</v>
@@ -4564,7 +4565,7 @@
         <v>45236</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -4578,16 +4579,16 @@
         <v>45210</v>
       </c>
       <c r="D75" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="G75" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="H75" s="4">
         <v>684.27</v>
@@ -4599,7 +4600,7 @@
         <v>45236</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -4613,16 +4614,16 @@
         <v>45210</v>
       </c>
       <c r="D76" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F76" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="H76" s="4">
         <v>626.79</v>
@@ -4634,7 +4635,7 @@
         <v>45236</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -4647,6 +4648,7 @@
     <hyperlink ref="K6" r:id="rId5" xr:uid="{F667B957-6845-4FAC-A527-A8016C4772C2}"/>
     <hyperlink ref="K4" r:id="rId6" xr:uid="{F6DBB2CC-913F-4D8F-B3F6-AE7014BCF2E3}"/>
     <hyperlink ref="K3" r:id="rId7" xr:uid="{4AAF3CF8-9906-4998-8E72-B74B4315D10F}"/>
+    <hyperlink ref="K9" r:id="rId8" xr:uid="{3F57EEB6-3EA6-45C4-A964-6995F699D159}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>